<commit_message>
add new exercises, section, definitions, fix typos, etc.
- fixed typos in lesson-14/literacy-7. (2nd ed.)
- updated anki deck/wordlist for Lesson 14. (3rd ed.)
- added new section for Lesson 15. (3rd ed.)
- added new dictionary definitions and updated existing ones.
- added the following exercises.

# Lesson 14 (3rd ed.)
- Kanji Vocabulary: 彼, 代, and 留
- Kanji Vocabulary: 族, 親, and 切
- Kanji Vocabulary: 英, 店, and 去
- Kanji Vocabulary: 急, 乗, and 当
- Kanji Vocabulary: 音, 楽, 医, and 者
- Kanji Practice: Write the Readings
- Reading Practice: 悩みの相談
- Workbook: Kanji Writing Practice
- Workbook: Using Kanji
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1069,6 +1069,798 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>he; boyfriend</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>彼|かれ</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>she; girlfriend</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>彼女|かのじょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>they</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>彼ら|かれら</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>boyfriend</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>彼氏|かれし</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>age; era</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>時代|じだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>electricity fee</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>電気代|でんきだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>90's</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>九十年代|きゅうじゅうねんだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>in one's teens</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>十代|じゅうだい</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>instead</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>代わりに|かわりに</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>international students</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>留学生|りゅうがくせい</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>to study abroad</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>留学する|りゅうがくする</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>absence; not home</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>留守|るす</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>family</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>家族|かぞく</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>race; ethnic group</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>民族|みんぞく</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>aquarium</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>水族館|すいぞくかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>member of royalty</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>王族|おうぞく</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>father</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>父親|ちちおや</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>親切な|しんせつな</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>best friend</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>親友|しんゆう</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>parents</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>両親|りょうしん</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>intimate</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>親しい|したしい</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>mother</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>母親|ははおや</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>to cut</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>切る|きる</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ticket</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>切符|きっぷ</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>postage stamp</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>切手|きって</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>precious</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>大切な|たいせつな</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>English language</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>英語|えいご</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>英国|えいこく</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>English conversation</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>英会話|えいかいわ</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>hero</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>英雄|えいゆう</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>shop</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>店|みせ</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>store clerk</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>店員|てんいん</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>stall; kiosk</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>売店|ばいてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>book store</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>書店|しょてん</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>store manager</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>店長|てんちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>last year</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>去年|きょねん</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>the past</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>過去|かこ</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>to leave</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>去る|さる</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>to erase</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>消去する|しょうきょする</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>suddenly</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>急に|きゅうに</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>to hurry</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>急ぐ|いそぐ</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>express train</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>急行|きゅうこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>super express</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>特急|とっきゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>to ride</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>乗る|のる</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>vehicle</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>乗り物|のりもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>riding a car</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>乗車|じょうしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>horseback riding</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>乗馬|じょうば</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>really</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>本当に|ほんとうに</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>lunch box</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>お弁当|おべんとう</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>at that time</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>当時|とうじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>to hit</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>当たる|あたる</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>music</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>音楽|おんがく</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>pronunciation</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>発音|はつおん</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>sound</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>音|おと</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>real intention</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>本音|ほんね</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>fun</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>楽しい|たのしい</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>musical instrument</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>楽器|がっき</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>easy; comfortable</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>楽な|らくな</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>doctor</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>医者|いしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>dentist</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>歯医者|はいしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>medical science</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>医学|いがく</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>clinic</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>医院|いいん</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>scholar</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>学者|がくしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>reader</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>読者|どくしゃ</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>young people</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>若者|わかもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>ninja</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>忍者|にんじゃ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update decks and wordlists
- updates the decks according to #260 in an attempt to fix the order.
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
@@ -700,7 +700,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>résumé</t>
+          <t>resume; résumé</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>I am no sure...</t>
+          <t>I am not sure...</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">

</xml_diff>